<commit_message>
Add support for csv exported from both 'Transaksjonsoversikt' and 'Søk i Transaksjoner' rather than just 'Transaksjonsoversikt' Bug fixes
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BBA5EA-54AF-46FC-A1EC-C29D47742AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D228D-E635-4C83-BCFF-A8C1CE377232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,7 +831,7 @@
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="9">
-        <f>D6-E6</f>
+        <f>E6-D6</f>
         <v>0</v>
       </c>
       <c r="H6" s="2"/>

</xml_diff>

<commit_message>
Add loading text on startup
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D228D-E635-4C83-BCFF-A8C1CE377232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57816AC-A7F7-47BE-9BE2-95A9CBFB1938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -842,7 +842,7 @@
     <col min="4" max="4" width="13.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="2.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="60.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="4.109375" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Minor adjustments to template Edit README
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\python_script\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57816AC-A7F7-47BE-9BE2-95A9CBFB1938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF79FEF0-C2E2-49E6-BA00-94B61E242877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>÷ Utstyr</t>
   </si>
   <si>
-    <t>÷ Utstyr til filterkvelder</t>
-  </si>
-  <si>
     <t>÷ Lederkvelder</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>FYLL INN</t>
+  </si>
+  <si>
+    <t>÷ Utgifter til filterkvelder</t>
   </si>
 </sst>
 </file>
@@ -828,11 +828,7 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -842,7 +838,7 @@
     <col min="4" max="4" width="13.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="2.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="60.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="4.109375" style="4" customWidth="1"/>
@@ -851,12 +847,12 @@
     <col min="13" max="16384" width="11.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
@@ -883,13 +879,13 @@
         <v>3</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J2" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" s="40" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -919,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="3"/>
@@ -942,7 +938,7 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="6"/>
       <c r="H5" s="2"/>
@@ -977,24 +973,24 @@
     </row>
     <row r="7" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1036,10 +1032,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="12"/>
     </row>
@@ -1289,7 +1285,7 @@
     <row r="25" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="str">
         <f>REPLACE(INDEX(UT,Kategorier!A10), 1, 2, "")</f>
-        <v>Utstyr til filterkvelder</v>
+        <v>Utgifter til filterkvelder</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="17">
@@ -1365,7 +1361,7 @@
     </row>
     <row r="32" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="20" t="e">
         <f>C16+C3</f>
@@ -1406,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1518,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1533,7 +1529,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1541,7 +1537,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1549,7 +1545,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add Graphical user interface
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF79FEF0-C2E2-49E6-BA00-94B61E242877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55170E-EE69-43E0-B50E-D2A9F52BBBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,9 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1402,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Organize regnskapsprogram.py to use classes instead of arrays when handling transactions
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55170E-EE69-43E0-B50E-D2A9F52BBBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88CE6F4-3018-4C69-B054-9208C3942878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,6 +518,134 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TekstSylinder 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB4F1CB-CDAE-B68B-5457-6D5EEF5E0BE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5631180" y="327660"/>
+          <a:ext cx="2286000" cy="1310640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Hvis du legger til nye kategorier i regnerarket "Kategorier", sett in tomme rader i oversikten</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>til venstre, under inntekter</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> eller utgifter. D</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ra ned formlene, og så vil sammendraget oppdatere seg automatisk.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -828,9 +956,7 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1010,9 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBF28CE-3AC6-4D68-A5F3-A708FFB83CF7}">
   <dimension ref="B1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1397,6 +1521,7 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add option to set account name when creating new account Add icon to main window Some minor code restructuring
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88CE6F4-3018-4C69-B054-9208C3942878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB173A75-4B0E-4BD1-8BF7-730ED9736F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>til venstre, under inntekter</a:t>
+            <a:t>til venstre under inntekter</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -633,7 +633,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ra ned formlene, og så vil sammendraget oppdatere seg automatisk.</a:t>
+            <a:t>ra ned formlene, og så vil de nye kategoriene</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> legges til i </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sammendraget.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO"/>
@@ -1529,9 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Remove "Category OK" column and move formula to the formatting rule instead GUI bug fix
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2F02D0-1C6C-41F9-BB25-E091B105E493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F6D73-28F0-4E8B-B578-EAE97E01D435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Dato</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>ÅRSTALL</t>
-  </si>
-  <si>
-    <t>Kategori OK</t>
   </si>
   <si>
     <t>FYLL INN</t>
@@ -975,7 +972,7 @@
   <sheetPr codeName="Ark1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -989,14 +986,13 @@
     <col min="6" max="6" width="2.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="60.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.88671875" style="1"/>
+    <col min="9" max="9" width="4.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
@@ -1027,17 +1023,14 @@
       <c r="H2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="36" t="s">
-        <v>28</v>
+      <c r="I2" s="40" t="s">
+        <v>25</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>4</v>
       </c>
@@ -1048,11 +1041,10 @@
       <c r="F3" s="1"/>
       <c r="G3" s="37"/>
       <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-    </row>
-    <row r="4" spans="1:11" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="str">
         <f>CONCATENATE("01.01.", C1)</f>
         <v>01.01.ÅRSTALL</v>
@@ -1064,17 +1056,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="str">
         <f>CONCATENATE("31.12.", C1)</f>
         <v>31.12.ÅRSTALL</v>
@@ -1087,15 +1078,14 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="6"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
         <v>8</v>
       </c>
@@ -1116,11 +1106,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>22</v>
       </c>
@@ -1136,7 +1125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="34" t="s">
         <v>23</v>
@@ -1575,10 +1564,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1586,10 +1575,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1597,10 +1586,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1608,10 +1597,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1619,10 +1608,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1630,10 +1619,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1641,10 +1630,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1652,10 +1641,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1663,10 +1652,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1674,10 +1663,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1685,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1693,7 +1682,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add configuration file for building with pyinstaller Change program icon Bug fixes Minor changes to template
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F6D73-28F0-4E8B-B578-EAE97E01D435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32852EC-6DC3-4700-8D43-99EF4A1662A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -974,7 +974,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1445,7 +1445,7 @@
     <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="str">
         <f>REPLACE(INDEX(UT,Kategorier!A12), 1, 2, "")</f>
-        <v xml:space="preserve"> Gebyrer</v>
+        <v xml:space="preserve"> Diverse</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="17">
@@ -1457,7 +1457,7 @@
     <row r="28" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="str">
         <f>REPLACE(INDEX(UT,Kategorier!A13), 1, 2, "")</f>
-        <v xml:space="preserve"> Diverse</v>
+        <v xml:space="preserve"> Gebyrer</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="17">
@@ -1539,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1674,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1682,7 +1682,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Create installer for Windows Organize example input files
</commit_message>
<xml_diff>
--- a/template/Filterregnskap_template.xlsx
+++ b/template/Filterregnskap_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Filter\Div\python_script\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32852EC-6DC3-4700-8D43-99EF4A1662A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AA36EB-B7D9-4C53-9F41-96EC457F0D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -974,7 +974,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1539,9 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>